<commit_message>
Cleanup, comment rewrites, lint, additional xlsx test
</commit_message>
<xml_diff>
--- a/libs/hdf-converters/sample_jsons/attestations/attestations.xlsx
+++ b/libs/hdf-converters/sample_jsons/attestations/attestations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmoors/Documents/Work/heimdall2/libs/hdf-converters/sample_jsons/attestations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dmedina\DSCA-SAF\attest_fix\heimdall2\libs\hdf-converters\sample_jsons\attestations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629B8212-904F-6C47-83B8-22B4BF99029B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE21B1C-60B6-4BAD-9103-B68F934393F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="720" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2412" yWindow="1956" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attestations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>Control_ID</t>
   </si>
@@ -40,49 +40,40 @@
     <t>Updated_By</t>
   </si>
   <si>
-    <t>annually</t>
-  </si>
-  <si>
     <t>passed</t>
   </si>
   <si>
-    <t>John Doe, ISSO</t>
-  </si>
-  <si>
-    <t>semiannually</t>
-  </si>
-  <si>
-    <t>quarterly</t>
-  </si>
-  <si>
-    <t>monthly</t>
-  </si>
-  <si>
-    <t>every2weeks</t>
-  </si>
-  <si>
-    <t>weekly</t>
-  </si>
-  <si>
-    <t>The routine review through interview/examination attests to this control passing</t>
-  </si>
-  <si>
-    <t>V-72083</t>
-  </si>
-  <si>
-    <t>V-72085</t>
-  </si>
-  <si>
-    <t>V-72087</t>
-  </si>
-  <si>
-    <t>V-72219</t>
-  </si>
-  <si>
-    <t>V-72315</t>
-  </si>
-  <si>
-    <t>V-73163</t>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>SV-230221</t>
+  </si>
+  <si>
+    <t>This control passes according to this attestation</t>
+  </si>
+  <si>
+    <t>153d</t>
+  </si>
+  <si>
+    <t>2024-03-21T22:17:52.761Z</t>
+  </si>
+  <si>
+    <t>SV-230222</t>
+  </si>
+  <si>
+    <t>This control fails according to this attestation</t>
+  </si>
+  <si>
+    <t>V-73166</t>
+  </si>
+  <si>
+    <t>SV-230223</t>
   </si>
 </sst>
 </file>
@@ -631,9 +622,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -671,7 +662,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -777,7 +768,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -919,7 +910,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -927,22 +918,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="69" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -962,127 +953,188 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1">
+        <v>401769</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1">
-        <v>58171</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>36161</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>58171</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1">
+        <v>401769</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1">
+        <v>36161</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1">
+        <v>401769</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>36161</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1">
-        <v>58171</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
+        <v>401769</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1">
-        <v>36256</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
+        <v>36161</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1">
-        <v>58171</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1">
-        <v>58171</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
+      <c r="F10" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>